<commit_message>
Updated quotation, invoice and pdf logic
</commit_message>
<xml_diff>
--- a/data/customers.xlsx
+++ b/data/customers.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -488,7 +488,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Fahad Ahmed Mohammed</t>
+          <t>Fahad Ahmed Mohamed</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -517,6 +517,34 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Fahad Ahmed Mohammed</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr"/>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Abu Dhabi - Al Shamkha</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>2025-11-16</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Fix product price sync on selection change and resolve SessionState widget conflicts
</commit_message>
<xml_diff>
--- a/data/customers.xlsx
+++ b/data/customers.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -491,10 +491,8 @@
           <t>Fahad Ahmed Mohamed</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>0502992932</t>
-        </is>
+      <c r="B2" t="n">
+        <v>502992932</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -541,7 +539,93 @@
       <c r="I3" t="inlineStr"/>
       <c r="J3" t="inlineStr">
         <is>
+          <t>2025-11-18</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Gfgsfhwrth</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr"/>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Abu Dhabi - Al Shamkha</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr">
+        <is>
           <t>2025-11-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Gfcngh</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr"/>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Abu Dhabi - Al Shamkha</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>New</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>2025-11-17</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Fahad</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>502992932</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Abu Dhabi - Al Shamkha</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>New</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="inlineStr"/>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>2025-11-17</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add product cards export and image handling fixes
</commit_message>
<xml_diff>
--- a/data/customers.xlsx
+++ b/data/customers.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -629,6 +629,38 @@
         </is>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Mr Nader</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>0503535395</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Abu Dhabi - Al Shamkha</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>New</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>2025-11-19</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>